<commit_message>
Change dashes to underscores in preparation for shinyfilter
</commit_message>
<xml_diff>
--- a/data/figure_captions.xlsx
+++ b/data/figure_captions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sumailsyr-my.sharepoint.com/personal/wbgearty_syr_edu/Documents/AMNH/Schizomida/data/drawings_database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sumailsyr-my.sharepoint.com/personal/wbgearty_syr_edu/Documents/AMNH/Schizomida/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{9D608BA6-62F0-4E11-8111-4D4F1DFBA61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72BDDD21-A249-42D8-A1E0-DA1C1E288D29}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{9D608BA6-62F0-4E11-8111-4D4F1DFBA61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BABB68AE-257D-4B67-83D4-1531B313C2C3}"/>
   <bookViews>
-    <workbookView xWindow="41364" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{57A6251D-BFCE-41E2-8D9E-CB6431C178B7}"/>
+    <workbookView xWindow="41364" yWindow="-2700" windowWidth="30936" windowHeight="16776" xr2:uid="{57A6251D-BFCE-41E2-8D9E-CB6431C178B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,67 +110,67 @@
     <t>1. No elongation of opisthosoma (majority of species). 2. Extreme elongation of segment IX. This particular condition is found in a single species from Singapore (Bucinozomus hortuspalmarum). 3. Elongation of segments V/VI-XII. This is a rare condition and is found only in species from the New World.</t>
   </si>
   <si>
-    <t>Setation--base-</t>
-  </si>
-  <si>
     <t>Dimorphism</t>
   </si>
   <si>
-    <t>Dorsal-setation</t>
-  </si>
-  <si>
     <t>Elongation</t>
   </si>
   <si>
-    <t>Number-of-flagellomeres--female-</t>
-  </si>
-  <si>
-    <t>Small-teeth--fixed-finger-</t>
-  </si>
-  <si>
-    <t>Anterodorsal-margin--leg-IV-</t>
-  </si>
-  <si>
-    <t>Accessory-tooth--movable-finger-</t>
-  </si>
-  <si>
-    <t>Guard-tooth--movable-finger-</t>
-  </si>
-  <si>
-    <t>Number-of-lobes</t>
-  </si>
-  <si>
     <t>Setation</t>
   </si>
   <si>
     <t>Sex</t>
   </si>
   <si>
-    <t>State-of-gonopod</t>
-  </si>
-  <si>
-    <t>State-of-metapeltidium</t>
-  </si>
-  <si>
-    <t>State-of-vision</t>
-  </si>
-  <si>
-    <t>Setation--tergite-II-</t>
-  </si>
-  <si>
-    <t>Tergite-XII--posterodorsal-process</t>
-  </si>
-  <si>
-    <t>Tergite-XII--posterodorsal-process--shape-</t>
-  </si>
-  <si>
-    <t>Apical-process--trochanter-</t>
-  </si>
-  <si>
-    <t>Mesal-spur--trochanter-</t>
-  </si>
-  <si>
-    <t>Dorsal-shape--male-</t>
+    <t>Accessory_tooth__movable_finger_</t>
+  </si>
+  <si>
+    <t>Anterodorsal_margin__leg_IV_</t>
+  </si>
+  <si>
+    <t>Apical_process__trochanter_</t>
+  </si>
+  <si>
+    <t>Dorsal_setation</t>
+  </si>
+  <si>
+    <t>Dorsal_shape__male_</t>
+  </si>
+  <si>
+    <t>Guard_tooth__movable_finger_</t>
+  </si>
+  <si>
+    <t>Mesal_spur__trochanter_</t>
+  </si>
+  <si>
+    <t>Number_of_flagellomeres__female_</t>
+  </si>
+  <si>
+    <t>Number_of_lobes</t>
+  </si>
+  <si>
+    <t>Setation__base_</t>
+  </si>
+  <si>
+    <t>Setation__tergite_II_</t>
+  </si>
+  <si>
+    <t>Small_teeth__fixed_finger_</t>
+  </si>
+  <si>
+    <t>State_of_gonopod</t>
+  </si>
+  <si>
+    <t>State_of_metapeltidium</t>
+  </si>
+  <si>
+    <t>State_of_vision</t>
+  </si>
+  <si>
+    <t>Tergite_XII__posterodorsal_process</t>
+  </si>
+  <si>
+    <t>Tergite_XII__posterodorsal_process__shape_</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -544,7 +544,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -568,7 +568,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -576,7 +576,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -592,7 +592,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -600,7 +600,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -608,7 +608,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -624,7 +624,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -664,7 +664,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
@@ -680,7 +680,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -688,7 +688,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>

</xml_diff>